<commit_message>
Añado doc, seccion de ayuda y estilo principal para fichar
</commit_message>
<xml_diff>
--- a/doc/TimeTracking.xlsx
+++ b/doc/TimeTracking.xlsx
@@ -5,16 +5,17 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ivan.iglesias\Code\work_time_manager\doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ivan.iglesias\Code\time_tracking\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12000" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12000" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
     <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
-    <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
+    <sheet name="Hoja4" sheetId="4" r:id="rId3"/>
+    <sheet name="Hoja3" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -369,6 +370,8 @@
   </tableStyles>
   <colors>
     <mruColors>
+      <color rgb="FFEF8B47"/>
+      <color rgb="FFFF5353"/>
       <color rgb="FFCBA9E5"/>
     </mruColors>
   </colors>
@@ -384,6 +387,1236 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>495300</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>30040</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>515816</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>55685</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="70" name="Grupo 69"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="2019300" y="982540"/>
+          <a:ext cx="4592516" cy="4216645"/>
+          <a:chOff x="2209800" y="960560"/>
+          <a:chExt cx="4592516" cy="4216645"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="55" name="Rectángulo 54"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="3128596" y="3472961"/>
+            <a:ext cx="1135673" cy="234462"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:r>
+              <a:rPr lang="es-ES" sz="1000">
+                <a:solidFill>
+                  <a:schemeClr val="bg2">
+                    <a:lumMod val="25000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>Ausencia</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="es-ES" sz="1000" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="bg2">
+                    <a:lumMod val="25000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:rPr>
+              <a:t> normal</a:t>
+            </a:r>
+            <a:endParaRPr lang="es-ES" sz="1000">
+              <a:solidFill>
+                <a:schemeClr val="bg2">
+                  <a:lumMod val="25000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:endParaRPr>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="56" name="Rectángulo 55"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="5070234" y="2630364"/>
+            <a:ext cx="930518" cy="468923"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:r>
+              <a:rPr lang="es-ES" sz="1000">
+                <a:solidFill>
+                  <a:schemeClr val="bg2">
+                    <a:lumMod val="25000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>Ausencia</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="es-ES" sz="1000" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="bg2">
+                    <a:lumMod val="25000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:rPr>
+              <a:t> programada</a:t>
+            </a:r>
+            <a:endParaRPr lang="es-ES" sz="1000">
+              <a:solidFill>
+                <a:schemeClr val="bg2">
+                  <a:lumMod val="25000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:endParaRPr>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:grpSp>
+        <xdr:nvGrpSpPr>
+          <xdr:cNvPr id="69" name="Grupo 68"/>
+          <xdr:cNvGrpSpPr/>
+        </xdr:nvGrpSpPr>
+        <xdr:grpSpPr>
+          <a:xfrm>
+            <a:off x="2209800" y="960560"/>
+            <a:ext cx="4592516" cy="4216645"/>
+            <a:chOff x="2209800" y="960560"/>
+            <a:chExt cx="4592516" cy="4216645"/>
+          </a:xfrm>
+        </xdr:grpSpPr>
+        <xdr:cxnSp macro="">
+          <xdr:nvCxnSpPr>
+            <xdr:cNvPr id="21" name="Conector recto de flecha 20"/>
+            <xdr:cNvCxnSpPr>
+              <a:stCxn id="9" idx="2"/>
+              <a:endCxn id="7" idx="0"/>
+            </xdr:cNvCxnSpPr>
+          </xdr:nvCxnSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="3128963" y="1693985"/>
+              <a:ext cx="0" cy="391991"/>
+            </a:xfrm>
+            <a:prstGeom prst="straightConnector1">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:ln w="25400">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="50000"/>
+                  <a:lumOff val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:tailEnd type="triangle"/>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="1">
+              <a:schemeClr val="accent1"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:schemeClr val="accent1"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:schemeClr val="accent1"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+        </xdr:cxnSp>
+        <xdr:cxnSp macro="">
+          <xdr:nvCxnSpPr>
+            <xdr:cNvPr id="36" name="Conector angular 35"/>
+            <xdr:cNvCxnSpPr>
+              <a:stCxn id="4" idx="3"/>
+              <a:endCxn id="18" idx="2"/>
+            </xdr:cNvCxnSpPr>
+          </xdr:nvCxnSpPr>
+          <xdr:spPr>
+            <a:xfrm flipV="1">
+              <a:off x="3893527" y="2500678"/>
+              <a:ext cx="1989627" cy="556847"/>
+            </a:xfrm>
+            <a:prstGeom prst="bentConnector2">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:ln w="25400">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="50000"/>
+                  <a:lumOff val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:tailEnd type="triangle"/>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="1">
+              <a:schemeClr val="accent1"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:schemeClr val="accent1"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:schemeClr val="accent1"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+        </xdr:cxnSp>
+        <xdr:grpSp>
+          <xdr:nvGrpSpPr>
+            <xdr:cNvPr id="68" name="Grupo 67"/>
+            <xdr:cNvGrpSpPr/>
+          </xdr:nvGrpSpPr>
+          <xdr:grpSpPr>
+            <a:xfrm>
+              <a:off x="2209800" y="960560"/>
+              <a:ext cx="4592516" cy="4216645"/>
+              <a:chOff x="2209800" y="960560"/>
+              <a:chExt cx="4592516" cy="4216645"/>
+            </a:xfrm>
+          </xdr:grpSpPr>
+          <xdr:cxnSp macro="">
+            <xdr:nvCxnSpPr>
+              <xdr:cNvPr id="24" name="Conector angular 23"/>
+              <xdr:cNvCxnSpPr>
+                <a:stCxn id="3" idx="1"/>
+                <a:endCxn id="9" idx="1"/>
+              </xdr:cNvCxnSpPr>
+            </xdr:nvCxnSpPr>
+            <xdr:spPr>
+              <a:xfrm rot="10800000">
+                <a:off x="2209801" y="1327274"/>
+                <a:ext cx="150203" cy="1130177"/>
+              </a:xfrm>
+              <a:prstGeom prst="bentConnector3">
+                <a:avLst>
+                  <a:gd name="adj1" fmla="val 252194"/>
+                </a:avLst>
+              </a:prstGeom>
+              <a:ln w="25400">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="50000"/>
+                    <a:lumOff val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:tailEnd type="triangle"/>
+              </a:ln>
+            </xdr:spPr>
+            <xdr:style>
+              <a:lnRef idx="1">
+                <a:schemeClr val="accent1"/>
+              </a:lnRef>
+              <a:fillRef idx="0">
+                <a:schemeClr val="accent1"/>
+              </a:fillRef>
+              <a:effectRef idx="0">
+                <a:schemeClr val="accent1"/>
+              </a:effectRef>
+              <a:fontRef idx="minor">
+                <a:schemeClr val="tx1"/>
+              </a:fontRef>
+            </xdr:style>
+          </xdr:cxnSp>
+          <xdr:cxnSp macro="">
+            <xdr:nvCxnSpPr>
+              <xdr:cNvPr id="27" name="Conector recto de flecha 26"/>
+              <xdr:cNvCxnSpPr>
+                <a:stCxn id="4" idx="2"/>
+                <a:endCxn id="34" idx="0"/>
+              </xdr:cNvCxnSpPr>
+            </xdr:nvCxnSpPr>
+            <xdr:spPr>
+              <a:xfrm>
+                <a:off x="3126765" y="3276599"/>
+                <a:ext cx="5129" cy="548057"/>
+              </a:xfrm>
+              <a:prstGeom prst="straightConnector1">
+                <a:avLst/>
+              </a:prstGeom>
+              <a:ln w="25400">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="50000"/>
+                    <a:lumOff val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:tailEnd type="triangle"/>
+              </a:ln>
+            </xdr:spPr>
+            <xdr:style>
+              <a:lnRef idx="1">
+                <a:schemeClr val="accent1"/>
+              </a:lnRef>
+              <a:fillRef idx="0">
+                <a:schemeClr val="accent1"/>
+              </a:fillRef>
+              <a:effectRef idx="0">
+                <a:schemeClr val="accent1"/>
+              </a:effectRef>
+              <a:fontRef idx="minor">
+                <a:schemeClr val="tx1"/>
+              </a:fontRef>
+            </xdr:style>
+          </xdr:cxnSp>
+          <xdr:cxnSp macro="">
+            <xdr:nvCxnSpPr>
+              <xdr:cNvPr id="44" name="Conector angular 43"/>
+              <xdr:cNvCxnSpPr>
+                <a:stCxn id="32" idx="1"/>
+                <a:endCxn id="9" idx="1"/>
+              </xdr:cNvCxnSpPr>
+            </xdr:nvCxnSpPr>
+            <xdr:spPr>
+              <a:xfrm rot="10800000">
+                <a:off x="2209800" y="1327274"/>
+                <a:ext cx="153134" cy="3469671"/>
+              </a:xfrm>
+              <a:prstGeom prst="bentConnector3">
+                <a:avLst>
+                  <a:gd name="adj1" fmla="val 507652"/>
+                </a:avLst>
+              </a:prstGeom>
+              <a:ln w="25400">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="50000"/>
+                    <a:lumOff val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:tailEnd type="triangle"/>
+              </a:ln>
+            </xdr:spPr>
+            <xdr:style>
+              <a:lnRef idx="1">
+                <a:schemeClr val="accent1"/>
+              </a:lnRef>
+              <a:fillRef idx="0">
+                <a:schemeClr val="accent1"/>
+              </a:fillRef>
+              <a:effectRef idx="0">
+                <a:schemeClr val="accent1"/>
+              </a:effectRef>
+              <a:fontRef idx="minor">
+                <a:schemeClr val="tx1"/>
+              </a:fontRef>
+            </xdr:style>
+          </xdr:cxnSp>
+          <xdr:cxnSp macro="">
+            <xdr:nvCxnSpPr>
+              <xdr:cNvPr id="48" name="Conector angular 47"/>
+              <xdr:cNvCxnSpPr>
+                <a:stCxn id="33" idx="1"/>
+                <a:endCxn id="7" idx="1"/>
+              </xdr:cNvCxnSpPr>
+            </xdr:nvCxnSpPr>
+            <xdr:spPr>
+              <a:xfrm rot="10800000">
+                <a:off x="2209800" y="2762251"/>
+                <a:ext cx="153134" cy="1462448"/>
+              </a:xfrm>
+              <a:prstGeom prst="bentConnector3">
+                <a:avLst>
+                  <a:gd name="adj1" fmla="val 316266"/>
+                </a:avLst>
+              </a:prstGeom>
+              <a:ln w="25400">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="50000"/>
+                    <a:lumOff val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:tailEnd type="triangle"/>
+              </a:ln>
+            </xdr:spPr>
+            <xdr:style>
+              <a:lnRef idx="1">
+                <a:schemeClr val="accent1"/>
+              </a:lnRef>
+              <a:fillRef idx="0">
+                <a:schemeClr val="accent1"/>
+              </a:fillRef>
+              <a:effectRef idx="0">
+                <a:schemeClr val="accent1"/>
+              </a:effectRef>
+              <a:fontRef idx="minor">
+                <a:schemeClr val="tx1"/>
+              </a:fontRef>
+            </xdr:style>
+          </xdr:cxnSp>
+          <xdr:grpSp>
+            <xdr:nvGrpSpPr>
+              <xdr:cNvPr id="67" name="Grupo 66"/>
+              <xdr:cNvGrpSpPr/>
+            </xdr:nvGrpSpPr>
+            <xdr:grpSpPr>
+              <a:xfrm>
+                <a:off x="2209800" y="960560"/>
+                <a:ext cx="4592516" cy="4216645"/>
+                <a:chOff x="2209800" y="960560"/>
+                <a:chExt cx="4592516" cy="4216645"/>
+              </a:xfrm>
+            </xdr:grpSpPr>
+            <xdr:grpSp>
+              <xdr:nvGrpSpPr>
+                <xdr:cNvPr id="8" name="Grupo 7"/>
+                <xdr:cNvGrpSpPr/>
+              </xdr:nvGrpSpPr>
+              <xdr:grpSpPr>
+                <a:xfrm>
+                  <a:off x="2209800" y="2085976"/>
+                  <a:ext cx="1838325" cy="1352549"/>
+                  <a:chOff x="2095500" y="1809751"/>
+                  <a:chExt cx="1838325" cy="1352549"/>
+                </a:xfrm>
+              </xdr:grpSpPr>
+              <xdr:sp macro="" textlink="">
+                <xdr:nvSpPr>
+                  <xdr:cNvPr id="3" name="Rectángulo 2"/>
+                  <xdr:cNvSpPr/>
+                </xdr:nvSpPr>
+                <xdr:spPr>
+                  <a:xfrm>
+                    <a:off x="2245703" y="1962150"/>
+                    <a:ext cx="1533524" cy="438149"/>
+                  </a:xfrm>
+                  <a:prstGeom prst="rect">
+                    <a:avLst/>
+                  </a:prstGeom>
+                  <a:solidFill>
+                    <a:srgbClr val="FF5353"/>
+                  </a:solidFill>
+                  <a:ln>
+                    <a:noFill/>
+                  </a:ln>
+                </xdr:spPr>
+                <xdr:style>
+                  <a:lnRef idx="2">
+                    <a:schemeClr val="accent1">
+                      <a:shade val="50000"/>
+                    </a:schemeClr>
+                  </a:lnRef>
+                  <a:fillRef idx="1">
+                    <a:schemeClr val="accent1"/>
+                  </a:fillRef>
+                  <a:effectRef idx="0">
+                    <a:schemeClr val="accent1"/>
+                  </a:effectRef>
+                  <a:fontRef idx="minor">
+                    <a:schemeClr val="lt1"/>
+                  </a:fontRef>
+                </xdr:style>
+                <xdr:txBody>
+                  <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:pPr algn="ctr"/>
+                    <a:r>
+                      <a:rPr lang="es-ES" sz="1400" b="0">
+                        <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+                        <a:cs typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+                      </a:rPr>
+                      <a:t>Check Out</a:t>
+                    </a:r>
+                  </a:p>
+                </xdr:txBody>
+              </xdr:sp>
+              <xdr:sp macro="" textlink="">
+                <xdr:nvSpPr>
+                  <xdr:cNvPr id="4" name="Rectángulo 3"/>
+                  <xdr:cNvSpPr/>
+                </xdr:nvSpPr>
+                <xdr:spPr>
+                  <a:xfrm>
+                    <a:off x="2245703" y="2562225"/>
+                    <a:ext cx="1533524" cy="438149"/>
+                  </a:xfrm>
+                  <a:prstGeom prst="rect">
+                    <a:avLst/>
+                  </a:prstGeom>
+                  <a:solidFill>
+                    <a:srgbClr val="EF8B47"/>
+                  </a:solidFill>
+                  <a:ln>
+                    <a:noFill/>
+                  </a:ln>
+                </xdr:spPr>
+                <xdr:style>
+                  <a:lnRef idx="2">
+                    <a:schemeClr val="accent1">
+                      <a:shade val="50000"/>
+                    </a:schemeClr>
+                  </a:lnRef>
+                  <a:fillRef idx="1">
+                    <a:schemeClr val="accent1"/>
+                  </a:fillRef>
+                  <a:effectRef idx="0">
+                    <a:schemeClr val="accent1"/>
+                  </a:effectRef>
+                  <a:fontRef idx="minor">
+                    <a:schemeClr val="lt1"/>
+                  </a:fontRef>
+                </xdr:style>
+                <xdr:txBody>
+                  <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:pPr algn="ctr"/>
+                    <a:r>
+                      <a:rPr lang="es-ES" sz="1400" b="0">
+                        <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+                        <a:cs typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+                      </a:rPr>
+                      <a:t>Ausencia</a:t>
+                    </a:r>
+                  </a:p>
+                </xdr:txBody>
+              </xdr:sp>
+              <xdr:sp macro="" textlink="">
+                <xdr:nvSpPr>
+                  <xdr:cNvPr id="7" name="Rectángulo 6"/>
+                  <xdr:cNvSpPr/>
+                </xdr:nvSpPr>
+                <xdr:spPr>
+                  <a:xfrm>
+                    <a:off x="2095500" y="1809751"/>
+                    <a:ext cx="1838325" cy="1352549"/>
+                  </a:xfrm>
+                  <a:prstGeom prst="rect">
+                    <a:avLst/>
+                  </a:prstGeom>
+                  <a:noFill/>
+                  <a:ln w="15875">
+                    <a:solidFill>
+                      <a:schemeClr val="bg2">
+                        <a:lumMod val="50000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                  </a:ln>
+                </xdr:spPr>
+                <xdr:style>
+                  <a:lnRef idx="2">
+                    <a:schemeClr val="accent1">
+                      <a:shade val="50000"/>
+                    </a:schemeClr>
+                  </a:lnRef>
+                  <a:fillRef idx="1">
+                    <a:schemeClr val="accent1"/>
+                  </a:fillRef>
+                  <a:effectRef idx="0">
+                    <a:schemeClr val="accent1"/>
+                  </a:effectRef>
+                  <a:fontRef idx="minor">
+                    <a:schemeClr val="lt1"/>
+                  </a:fontRef>
+                </xdr:style>
+                <xdr:txBody>
+                  <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:pPr algn="l"/>
+                    <a:endParaRPr lang="es-ES" sz="1100"/>
+                  </a:p>
+                </xdr:txBody>
+              </xdr:sp>
+            </xdr:grpSp>
+            <xdr:grpSp>
+              <xdr:nvGrpSpPr>
+                <xdr:cNvPr id="10" name="Grupo 9"/>
+                <xdr:cNvGrpSpPr/>
+              </xdr:nvGrpSpPr>
+              <xdr:grpSpPr>
+                <a:xfrm>
+                  <a:off x="2209800" y="960560"/>
+                  <a:ext cx="1838325" cy="733425"/>
+                  <a:chOff x="2486025" y="438150"/>
+                  <a:chExt cx="1838325" cy="733425"/>
+                </a:xfrm>
+              </xdr:grpSpPr>
+              <xdr:sp macro="" textlink="">
+                <xdr:nvSpPr>
+                  <xdr:cNvPr id="2" name="Rectángulo 1"/>
+                  <xdr:cNvSpPr/>
+                </xdr:nvSpPr>
+                <xdr:spPr>
+                  <a:xfrm>
+                    <a:off x="2638427" y="581026"/>
+                    <a:ext cx="1533524" cy="438149"/>
+                  </a:xfrm>
+                  <a:prstGeom prst="rect">
+                    <a:avLst/>
+                  </a:prstGeom>
+                  <a:solidFill>
+                    <a:schemeClr val="accent6"/>
+                  </a:solidFill>
+                  <a:ln>
+                    <a:noFill/>
+                  </a:ln>
+                </xdr:spPr>
+                <xdr:style>
+                  <a:lnRef idx="2">
+                    <a:schemeClr val="accent1">
+                      <a:shade val="50000"/>
+                    </a:schemeClr>
+                  </a:lnRef>
+                  <a:fillRef idx="1">
+                    <a:schemeClr val="accent1"/>
+                  </a:fillRef>
+                  <a:effectRef idx="0">
+                    <a:schemeClr val="accent1"/>
+                  </a:effectRef>
+                  <a:fontRef idx="minor">
+                    <a:schemeClr val="lt1"/>
+                  </a:fontRef>
+                </xdr:style>
+                <xdr:txBody>
+                  <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:pPr algn="ctr"/>
+                    <a:r>
+                      <a:rPr lang="es-ES" sz="1400" b="0">
+                        <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+                        <a:cs typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+                      </a:rPr>
+                      <a:t>Check In</a:t>
+                    </a:r>
+                  </a:p>
+                </xdr:txBody>
+              </xdr:sp>
+              <xdr:sp macro="" textlink="">
+                <xdr:nvSpPr>
+                  <xdr:cNvPr id="9" name="Rectángulo 8"/>
+                  <xdr:cNvSpPr/>
+                </xdr:nvSpPr>
+                <xdr:spPr>
+                  <a:xfrm>
+                    <a:off x="2486025" y="438150"/>
+                    <a:ext cx="1838325" cy="733425"/>
+                  </a:xfrm>
+                  <a:prstGeom prst="rect">
+                    <a:avLst/>
+                  </a:prstGeom>
+                  <a:noFill/>
+                  <a:ln w="15875">
+                    <a:solidFill>
+                      <a:schemeClr val="bg2">
+                        <a:lumMod val="50000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                  </a:ln>
+                </xdr:spPr>
+                <xdr:style>
+                  <a:lnRef idx="2">
+                    <a:schemeClr val="accent1">
+                      <a:shade val="50000"/>
+                    </a:schemeClr>
+                  </a:lnRef>
+                  <a:fillRef idx="1">
+                    <a:schemeClr val="accent1"/>
+                  </a:fillRef>
+                  <a:effectRef idx="0">
+                    <a:schemeClr val="accent1"/>
+                  </a:effectRef>
+                  <a:fontRef idx="minor">
+                    <a:schemeClr val="lt1"/>
+                  </a:fontRef>
+                </xdr:style>
+                <xdr:txBody>
+                  <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:pPr algn="l"/>
+                    <a:endParaRPr lang="es-ES" sz="1100"/>
+                  </a:p>
+                </xdr:txBody>
+              </xdr:sp>
+            </xdr:grpSp>
+            <xdr:grpSp>
+              <xdr:nvGrpSpPr>
+                <xdr:cNvPr id="19" name="Grupo 18"/>
+                <xdr:cNvGrpSpPr/>
+              </xdr:nvGrpSpPr>
+              <xdr:grpSpPr>
+                <a:xfrm>
+                  <a:off x="4963991" y="1767253"/>
+                  <a:ext cx="1838325" cy="733425"/>
+                  <a:chOff x="5334000" y="1905000"/>
+                  <a:chExt cx="1838325" cy="733425"/>
+                </a:xfrm>
+              </xdr:grpSpPr>
+              <xdr:sp macro="" textlink="">
+                <xdr:nvSpPr>
+                  <xdr:cNvPr id="6" name="Rectángulo 5"/>
+                  <xdr:cNvSpPr/>
+                </xdr:nvSpPr>
+                <xdr:spPr>
+                  <a:xfrm>
+                    <a:off x="5476876" y="2047875"/>
+                    <a:ext cx="1533524" cy="438149"/>
+                  </a:xfrm>
+                  <a:prstGeom prst="rect">
+                    <a:avLst/>
+                  </a:prstGeom>
+                  <a:solidFill>
+                    <a:srgbClr val="C00000"/>
+                  </a:solidFill>
+                  <a:ln>
+                    <a:noFill/>
+                  </a:ln>
+                </xdr:spPr>
+                <xdr:style>
+                  <a:lnRef idx="2">
+                    <a:schemeClr val="accent1">
+                      <a:shade val="50000"/>
+                    </a:schemeClr>
+                  </a:lnRef>
+                  <a:fillRef idx="1">
+                    <a:schemeClr val="accent1"/>
+                  </a:fillRef>
+                  <a:effectRef idx="0">
+                    <a:schemeClr val="accent1"/>
+                  </a:effectRef>
+                  <a:fontRef idx="minor">
+                    <a:schemeClr val="lt1"/>
+                  </a:fontRef>
+                </xdr:style>
+                <xdr:txBody>
+                  <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:pPr algn="ctr"/>
+                    <a:r>
+                      <a:rPr lang="es-ES" sz="1400" b="0">
+                        <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+                        <a:cs typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+                      </a:rPr>
+                      <a:t>Cancelar Ausencia</a:t>
+                    </a:r>
+                  </a:p>
+                </xdr:txBody>
+              </xdr:sp>
+              <xdr:sp macro="" textlink="">
+                <xdr:nvSpPr>
+                  <xdr:cNvPr id="18" name="Rectángulo 17"/>
+                  <xdr:cNvSpPr/>
+                </xdr:nvSpPr>
+                <xdr:spPr>
+                  <a:xfrm>
+                    <a:off x="5334000" y="1905000"/>
+                    <a:ext cx="1838325" cy="733425"/>
+                  </a:xfrm>
+                  <a:prstGeom prst="rect">
+                    <a:avLst/>
+                  </a:prstGeom>
+                  <a:noFill/>
+                  <a:ln w="15875">
+                    <a:solidFill>
+                      <a:schemeClr val="bg2">
+                        <a:lumMod val="50000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                  </a:ln>
+                </xdr:spPr>
+                <xdr:style>
+                  <a:lnRef idx="2">
+                    <a:schemeClr val="accent1">
+                      <a:shade val="50000"/>
+                    </a:schemeClr>
+                  </a:lnRef>
+                  <a:fillRef idx="1">
+                    <a:schemeClr val="accent1"/>
+                  </a:fillRef>
+                  <a:effectRef idx="0">
+                    <a:schemeClr val="accent1"/>
+                  </a:effectRef>
+                  <a:fontRef idx="minor">
+                    <a:schemeClr val="lt1"/>
+                  </a:fontRef>
+                </xdr:style>
+                <xdr:txBody>
+                  <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:pPr algn="l"/>
+                    <a:endParaRPr lang="es-ES" sz="1100"/>
+                  </a:p>
+                </xdr:txBody>
+              </xdr:sp>
+            </xdr:grpSp>
+            <xdr:grpSp>
+              <xdr:nvGrpSpPr>
+                <xdr:cNvPr id="31" name="Grupo 30"/>
+                <xdr:cNvGrpSpPr/>
+              </xdr:nvGrpSpPr>
+              <xdr:grpSpPr>
+                <a:xfrm>
+                  <a:off x="2212731" y="3824656"/>
+                  <a:ext cx="1838325" cy="1352549"/>
+                  <a:chOff x="2095500" y="1809751"/>
+                  <a:chExt cx="1838325" cy="1352549"/>
+                </a:xfrm>
+              </xdr:grpSpPr>
+              <xdr:sp macro="" textlink="">
+                <xdr:nvSpPr>
+                  <xdr:cNvPr id="32" name="Rectángulo 31"/>
+                  <xdr:cNvSpPr/>
+                </xdr:nvSpPr>
+                <xdr:spPr>
+                  <a:xfrm>
+                    <a:off x="2245703" y="2562964"/>
+                    <a:ext cx="1533524" cy="438149"/>
+                  </a:xfrm>
+                  <a:prstGeom prst="rect">
+                    <a:avLst/>
+                  </a:prstGeom>
+                  <a:solidFill>
+                    <a:srgbClr val="FF5353"/>
+                  </a:solidFill>
+                  <a:ln>
+                    <a:noFill/>
+                  </a:ln>
+                </xdr:spPr>
+                <xdr:style>
+                  <a:lnRef idx="2">
+                    <a:schemeClr val="accent1">
+                      <a:shade val="50000"/>
+                    </a:schemeClr>
+                  </a:lnRef>
+                  <a:fillRef idx="1">
+                    <a:schemeClr val="accent1"/>
+                  </a:fillRef>
+                  <a:effectRef idx="0">
+                    <a:schemeClr val="accent1"/>
+                  </a:effectRef>
+                  <a:fontRef idx="minor">
+                    <a:schemeClr val="lt1"/>
+                  </a:fontRef>
+                </xdr:style>
+                <xdr:txBody>
+                  <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:pPr algn="ctr"/>
+                    <a:r>
+                      <a:rPr lang="es-ES" sz="1400" b="0">
+                        <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+                        <a:cs typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+                      </a:rPr>
+                      <a:t>Check Out</a:t>
+                    </a:r>
+                  </a:p>
+                </xdr:txBody>
+              </xdr:sp>
+              <xdr:sp macro="" textlink="">
+                <xdr:nvSpPr>
+                  <xdr:cNvPr id="33" name="Rectángulo 32"/>
+                  <xdr:cNvSpPr/>
+                </xdr:nvSpPr>
+                <xdr:spPr>
+                  <a:xfrm>
+                    <a:off x="2245703" y="1990719"/>
+                    <a:ext cx="1533524" cy="438149"/>
+                  </a:xfrm>
+                  <a:prstGeom prst="rect">
+                    <a:avLst/>
+                  </a:prstGeom>
+                  <a:solidFill>
+                    <a:schemeClr val="accent2">
+                      <a:lumMod val="75000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:ln>
+                    <a:noFill/>
+                  </a:ln>
+                </xdr:spPr>
+                <xdr:style>
+                  <a:lnRef idx="2">
+                    <a:schemeClr val="accent1">
+                      <a:shade val="50000"/>
+                    </a:schemeClr>
+                  </a:lnRef>
+                  <a:fillRef idx="1">
+                    <a:schemeClr val="accent1"/>
+                  </a:fillRef>
+                  <a:effectRef idx="0">
+                    <a:schemeClr val="accent1"/>
+                  </a:effectRef>
+                  <a:fontRef idx="minor">
+                    <a:schemeClr val="lt1"/>
+                  </a:fontRef>
+                </xdr:style>
+                <xdr:txBody>
+                  <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:pPr algn="ctr"/>
+                    <a:r>
+                      <a:rPr lang="es-ES" sz="1400" b="0">
+                        <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+                        <a:cs typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+                      </a:rPr>
+                      <a:t>Terminar Ausencia</a:t>
+                    </a:r>
+                  </a:p>
+                </xdr:txBody>
+              </xdr:sp>
+              <xdr:sp macro="" textlink="">
+                <xdr:nvSpPr>
+                  <xdr:cNvPr id="34" name="Rectángulo 33"/>
+                  <xdr:cNvSpPr/>
+                </xdr:nvSpPr>
+                <xdr:spPr>
+                  <a:xfrm>
+                    <a:off x="2095500" y="1809751"/>
+                    <a:ext cx="1838325" cy="1352549"/>
+                  </a:xfrm>
+                  <a:prstGeom prst="rect">
+                    <a:avLst/>
+                  </a:prstGeom>
+                  <a:noFill/>
+                  <a:ln w="15875">
+                    <a:solidFill>
+                      <a:schemeClr val="bg2">
+                        <a:lumMod val="50000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                  </a:ln>
+                </xdr:spPr>
+                <xdr:style>
+                  <a:lnRef idx="2">
+                    <a:schemeClr val="accent1">
+                      <a:shade val="50000"/>
+                    </a:schemeClr>
+                  </a:lnRef>
+                  <a:fillRef idx="1">
+                    <a:schemeClr val="accent1"/>
+                  </a:fillRef>
+                  <a:effectRef idx="0">
+                    <a:schemeClr val="accent1"/>
+                  </a:effectRef>
+                  <a:fontRef idx="minor">
+                    <a:schemeClr val="lt1"/>
+                  </a:fontRef>
+                </xdr:style>
+                <xdr:txBody>
+                  <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:pPr algn="l"/>
+                    <a:endParaRPr lang="es-ES" sz="1100"/>
+                  </a:p>
+                </xdr:txBody>
+              </xdr:sp>
+            </xdr:grpSp>
+            <xdr:cxnSp macro="">
+              <xdr:nvCxnSpPr>
+                <xdr:cNvPr id="41" name="Conector angular 40"/>
+                <xdr:cNvCxnSpPr>
+                  <a:stCxn id="18" idx="0"/>
+                  <a:endCxn id="2" idx="3"/>
+                </xdr:cNvCxnSpPr>
+              </xdr:nvCxnSpPr>
+              <xdr:spPr>
+                <a:xfrm rot="16200000" flipV="1">
+                  <a:off x="4667069" y="551168"/>
+                  <a:ext cx="444742" cy="1987428"/>
+                </a:xfrm>
+                <a:prstGeom prst="bentConnector2">
+                  <a:avLst/>
+                </a:prstGeom>
+                <a:ln w="25400">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="50000"/>
+                      <a:lumOff val="50000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:tailEnd type="triangle"/>
+                </a:ln>
+              </xdr:spPr>
+              <xdr:style>
+                <a:lnRef idx="1">
+                  <a:schemeClr val="accent1"/>
+                </a:lnRef>
+                <a:fillRef idx="0">
+                  <a:schemeClr val="accent1"/>
+                </a:fillRef>
+                <a:effectRef idx="0">
+                  <a:schemeClr val="accent1"/>
+                </a:effectRef>
+                <a:fontRef idx="minor">
+                  <a:schemeClr val="tx1"/>
+                </a:fontRef>
+              </xdr:style>
+            </xdr:cxnSp>
+            <xdr:cxnSp macro="">
+              <xdr:nvCxnSpPr>
+                <xdr:cNvPr id="62" name="Conector angular 61"/>
+                <xdr:cNvCxnSpPr>
+                  <a:stCxn id="18" idx="1"/>
+                  <a:endCxn id="7" idx="3"/>
+                </xdr:cNvCxnSpPr>
+              </xdr:nvCxnSpPr>
+              <xdr:spPr>
+                <a:xfrm rot="10800000" flipV="1">
+                  <a:off x="4048125" y="2133965"/>
+                  <a:ext cx="915866" cy="628285"/>
+                </a:xfrm>
+                <a:prstGeom prst="bentConnector3">
+                  <a:avLst>
+                    <a:gd name="adj1" fmla="val 50000"/>
+                  </a:avLst>
+                </a:prstGeom>
+                <a:ln w="25400">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="50000"/>
+                      <a:lumOff val="50000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:tailEnd type="triangle"/>
+                </a:ln>
+              </xdr:spPr>
+              <xdr:style>
+                <a:lnRef idx="1">
+                  <a:schemeClr val="accent1"/>
+                </a:lnRef>
+                <a:fillRef idx="0">
+                  <a:schemeClr val="accent1"/>
+                </a:fillRef>
+                <a:effectRef idx="0">
+                  <a:schemeClr val="accent1"/>
+                </a:effectRef>
+                <a:fontRef idx="minor">
+                  <a:schemeClr val="tx1"/>
+                </a:fontRef>
+              </xdr:style>
+            </xdr:cxnSp>
+          </xdr:grpSp>
+        </xdr:grpSp>
+      </xdr:grpSp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="65" name="Rectángulo 64"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="4088422" y="1069731"/>
+            <a:ext cx="2161443" cy="468923"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:r>
+              <a:rPr lang="es-ES" sz="1000">
+                <a:solidFill>
+                  <a:schemeClr val="bg2">
+                    <a:lumMod val="25000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>Ausencia</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="es-ES" sz="1000" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="bg2">
+                    <a:lumMod val="25000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:rPr>
+              <a:t> Programada Terminada</a:t>
+            </a:r>
+            <a:endParaRPr lang="es-ES" sz="1000">
+              <a:solidFill>
+                <a:schemeClr val="bg2">
+                  <a:lumMod val="25000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:endParaRPr>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="66" name="Rectángulo 65"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="4293576" y="1890347"/>
+            <a:ext cx="703385" cy="315058"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:r>
+              <a:rPr lang="es-ES" sz="1000" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="bg2">
+                    <a:lumMod val="25000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>Cancelar</a:t>
+            </a:r>
+            <a:endParaRPr lang="es-ES" sz="1000">
+              <a:solidFill>
+                <a:schemeClr val="bg2">
+                  <a:lumMod val="25000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:endParaRPr>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -1181,7 +2414,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H31" sqref="H31"/>
     </sheetView>
   </sheetViews>
@@ -1687,10 +2920,25 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="M13" sqref="M13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="F13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+      <selection activeCell="L21" sqref="L21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>